<commit_message>
test: Test parameters Train25...26
</commit_message>
<xml_diff>
--- a/training_results/train_25_lr_hyper_param.xlsx
+++ b/training_results/train_25_lr_hyper_param.xlsx
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>128</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -482,7 +482,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.0001</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -490,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>